<commit_message>
working on service document support
</commit_message>
<xml_diff>
--- a/application/views/rpt/ua/doc/service_invoice.xlsx
+++ b/application/views/rpt/ua/doc/service_invoice.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>прийому-передачі виконаних робіт (наданих послуг)</t>
   </si>
@@ -103,9 +103,6 @@
     <t>{$v-&gt;doc_view-&gt;total_spell}</t>
   </si>
   <si>
-    <t xml:space="preserve"> {$v-&gt;doc_view-&gt;user_position} {$v-&gt;doc_view-&gt;user_sign}</t>
-  </si>
-  <si>
     <t>Виконавець</t>
   </si>
   <si>
@@ -121,7 +118,13 @@
     <t>Всього на суму:</t>
   </si>
   <si>
-    <t>Ми, що нижче підписалися, представник Виконавця і представник Замовника, уклали цей акт про те, що Виконавець виконав роботи (надав послуги) згідно договору №{$v-&gt;p-&gt;company_agreement_num} від {$v-&gt;p-&gt;ag_date_dot}.</t>
+    <t>Ми, що нижче підписалися, представник Виконавця і представник Замовника, уклали цей акт про те, що Виконавець виконав роботи (надав послуги) згідно договору №{$v-&gt;ag_num} від {$v-&gt;ag_date_dot}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {$v-&gt;sign_performer}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {$v-&gt;sign_customer}</t>
   </si>
 </sst>
 </file>
@@ -330,15 +333,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -362,30 +389,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,7 +755,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D4"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -769,85 +772,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="A3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
+      <c r="A6" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="6" t="s">
         <v>3</v>
       </c>
@@ -865,11 +868,11 @@
       <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="10" t="s">
         <v>18</v>
       </c>
@@ -887,10 +890,10 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="25"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="11" t="s">
         <v>22</v>
       </c>
@@ -899,10 +902,10 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="26"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="11" t="s">
         <v>23</v>
       </c>
@@ -911,10 +914,10 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="26"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="11" t="s">
         <v>24</v>
       </c>
@@ -929,18 +932,18 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23" t="s">
+      <c r="A13" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -952,42 +955,42 @@
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
     </row>
     <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
     </row>
     <row r="19" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -1001,33 +1004,30 @@
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="3"/>
       <c r="F20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="B21" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="F21" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="23">
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="B7:D7"/>
+  <mergeCells count="24">
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -1043,6 +1043,15 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>